<commit_message>
Uploading original Excel file
Empty Excel file containing only stock symbols.
</commit_message>
<xml_diff>
--- a/stocks_original.xlsx
+++ b/stocks_original.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fioyu\Desktop\StudioX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CEC766-946F-412E-A5B0-0E77710FE6AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129E2232-017A-4F3C-8704-3867F64B9866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B57C0270-149C-41C0-B438-A8502C2D986D}"/>
+    <workbookView xWindow="-24405" yWindow="435" windowWidth="21675" windowHeight="13050" xr2:uid="{B57C0270-149C-41C0-B438-A8502C2D986D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,29 +68,29 @@
     <t>RDZN</t>
   </si>
   <si>
-    <t>^HSI</t>
-  </si>
-  <si>
     <t>VS</t>
   </si>
   <si>
     <t>HFG.DE</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>P/E Ratio</t>
-  </si>
-  <si>
     <t>MarketCap</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>PERatio</t>
+  </si>
+  <si>
+    <t>EPS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +111,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,11 +140,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -474,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6598E499-276D-4F02-8993-AFCB0071E1A2}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G10" sqref="G10:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,132 +495,116 @@
     <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="H9" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A9" r:id="rId1" tooltip="Versus Systems Inc." display="https://finance.yahoo.com/quote/VS/" xr:uid="{ABB66CA8-1292-4CC1-90FA-ADC5F47830A0}"/>
-    <hyperlink ref="A10" r:id="rId2" tooltip="HelloFresh SE" display="https://finance.yahoo.com/quote/HFG.DE/" xr:uid="{FC17F5CD-EA5B-4874-997E-C139F1009AD2}"/>
+    <hyperlink ref="A8" r:id="rId1" tooltip="Versus Systems Inc." display="https://finance.yahoo.com/quote/VS/" xr:uid="{112FE6F2-EAEF-4581-90ED-1FC3389ABAA1}"/>
+    <hyperlink ref="A9" r:id="rId2" tooltip="HelloFresh SE" display="https://finance.yahoo.com/quote/HFG.DE/" xr:uid="{5799F733-7CCF-4B37-ADAB-3C7DE904CC81}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>